<commit_message>
Adding a boarder to the dashbaord
</commit_message>
<xml_diff>
--- a/Monetary_stats_1995-2023.xlsx
+++ b/Monetary_stats_1995-2023.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abirshanaa\Downloads\Web_data_-_October_-_December_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e372d3a2a585731b/Documents/IIT/IIT-second year/Second sem/Project lifecycle/Courseworks-DSPL/W2052147_Monetary-Trends/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831D2586-108A-4ABB-80A4-762546A89BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{831D2586-108A-4ABB-80A4-762546A89BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C82B114-B264-4959-AB23-1D5A1014C143}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4.02" sheetId="1" r:id="rId1"/>
     <sheet name="Compatibility Report" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'4.02'!$B$1:$D$354</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'4.02'!$A$1:$W$362</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -904,6 +905,9 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -912,9 +916,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1227,39 +1228,39 @@
   <dimension ref="A1:AO376"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="40" workbookViewId="0">
-      <pane xSplit="2" ySplit="5" topLeftCell="C349" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="5" topLeftCell="C347" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="O353" sqref="O353"/>
+      <selection pane="bottomRight" activeCell="B354" sqref="B6:B354"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="12.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="12.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="2" style="2" customWidth="1"/>
     <col min="6" max="6" width="14" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="2" customWidth="1"/>
-    <col min="8" max="8" width="14.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" style="2" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" style="2" customWidth="1"/>
     <col min="10" max="10" width="16" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="2" style="2" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="16.85546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="15.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="16.88671875" style="2" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="2" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="16.85546875" style="3" customWidth="1"/>
-    <col min="18" max="18" width="18.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="18.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.85546875" style="2" customWidth="1"/>
-    <col min="22" max="22" width="19.140625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="41" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="2"/>
+    <col min="16" max="16" width="16.109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="16.88671875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="18.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.33203125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.88671875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="19.109375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="19.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="41" width="14.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="42" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="18.75" x14ac:dyDescent="0.3">
@@ -1267,7 +1268,7 @@
         <v>4.0199999999999996</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C2" s="32" t="s">
         <v>5</v>
       </c>
@@ -1278,7 +1279,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="C3" s="33"/>
       <c r="D3" s="11" t="s">
         <v>6</v>
@@ -1290,13 +1291,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="5" customFormat="1" ht="82.5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" s="5" customFormat="1" ht="72" x14ac:dyDescent="0.3">
       <c r="A4" s="34"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="62" t="s">
+      <c r="D4" s="63" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="25"/>
@@ -1357,8 +1358,8 @@
     <row r="5" spans="1:41" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="34"/>
       <c r="B5" s="39"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
+      <c r="C5" s="64"/>
+      <c r="D5" s="64"/>
       <c r="E5" s="35"/>
       <c r="F5" s="1">
         <v>-1</v>
@@ -1410,7 +1411,7 @@
       <c r="W5" s="24"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B6" s="30">
         <v>35034</v>
       </c>
@@ -1498,7 +1499,7 @@
       <c r="AN6" s="8"/>
       <c r="AO6" s="8"/>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B7" s="30">
         <v>35065</v>
       </c>
@@ -1586,7 +1587,7 @@
       <c r="AN7" s="8"/>
       <c r="AO7" s="8"/>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="30">
         <v>35096</v>
       </c>
@@ -1674,7 +1675,7 @@
       <c r="AN8" s="8"/>
       <c r="AO8" s="8"/>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B9" s="30">
         <v>35125</v>
       </c>
@@ -1762,7 +1763,7 @@
       <c r="AN9" s="8"/>
       <c r="AO9" s="8"/>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="30">
         <v>35156</v>
       </c>
@@ -1850,7 +1851,7 @@
       <c r="AN10" s="8"/>
       <c r="AO10" s="8"/>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B11" s="30">
         <v>35186</v>
       </c>
@@ -1938,7 +1939,7 @@
       <c r="AN11" s="8"/>
       <c r="AO11" s="8"/>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B12" s="30">
         <v>35217</v>
       </c>
@@ -2026,7 +2027,7 @@
       <c r="AN12" s="8"/>
       <c r="AO12" s="8"/>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B13" s="30">
         <v>35247</v>
       </c>
@@ -2114,7 +2115,7 @@
       <c r="AN13" s="8"/>
       <c r="AO13" s="8"/>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B14" s="30">
         <v>35278</v>
       </c>
@@ -2202,7 +2203,7 @@
       <c r="AN14" s="8"/>
       <c r="AO14" s="8"/>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B15" s="30">
         <v>35309</v>
       </c>
@@ -2290,7 +2291,7 @@
       <c r="AN15" s="8"/>
       <c r="AO15" s="8"/>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B16" s="30">
         <v>35339</v>
       </c>
@@ -2378,7 +2379,7 @@
       <c r="AN16" s="8"/>
       <c r="AO16" s="8"/>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B17" s="30">
         <v>35370</v>
       </c>
@@ -2466,7 +2467,7 @@
       <c r="AN17" s="8"/>
       <c r="AO17" s="8"/>
     </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B18" s="30">
         <v>35400</v>
       </c>
@@ -2554,7 +2555,7 @@
       <c r="AN18" s="8"/>
       <c r="AO18" s="8"/>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B19" s="30">
         <v>35431</v>
       </c>
@@ -2642,7 +2643,7 @@
       <c r="AN19" s="8"/>
       <c r="AO19" s="8"/>
     </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B20" s="30">
         <v>35462</v>
       </c>
@@ -2730,7 +2731,7 @@
       <c r="AN20" s="8"/>
       <c r="AO20" s="8"/>
     </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B21" s="30">
         <v>35490</v>
       </c>
@@ -2818,7 +2819,7 @@
       <c r="AN21" s="8"/>
       <c r="AO21" s="8"/>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B22" s="30">
         <v>35521</v>
       </c>
@@ -2906,7 +2907,7 @@
       <c r="AN22" s="8"/>
       <c r="AO22" s="8"/>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B23" s="30">
         <v>35551</v>
       </c>
@@ -2994,7 +2995,7 @@
       <c r="AN23" s="8"/>
       <c r="AO23" s="8"/>
     </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B24" s="30">
         <v>35582</v>
       </c>
@@ -3082,7 +3083,7 @@
       <c r="AN24" s="8"/>
       <c r="AO24" s="8"/>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B25" s="30">
         <v>35612</v>
       </c>
@@ -3170,7 +3171,7 @@
       <c r="AN25" s="8"/>
       <c r="AO25" s="8"/>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B26" s="30">
         <v>35643</v>
       </c>
@@ -3258,7 +3259,7 @@
       <c r="AN26" s="8"/>
       <c r="AO26" s="8"/>
     </row>
-    <row r="27" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B27" s="30">
         <v>35674</v>
       </c>
@@ -3346,7 +3347,7 @@
       <c r="AN27" s="8"/>
       <c r="AO27" s="8"/>
     </row>
-    <row r="28" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B28" s="30">
         <v>35704</v>
       </c>
@@ -3434,7 +3435,7 @@
       <c r="AN28" s="8"/>
       <c r="AO28" s="8"/>
     </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B29" s="30">
         <v>35735</v>
       </c>
@@ -3522,7 +3523,7 @@
       <c r="AN29" s="8"/>
       <c r="AO29" s="8"/>
     </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B30" s="30">
         <v>35765</v>
       </c>
@@ -3610,7 +3611,7 @@
       <c r="AN30" s="8"/>
       <c r="AO30" s="8"/>
     </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B31" s="30">
         <v>35796</v>
       </c>
@@ -3698,7 +3699,7 @@
       <c r="AN31" s="8"/>
       <c r="AO31" s="8"/>
     </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B32" s="30">
         <v>35827</v>
       </c>
@@ -3786,7 +3787,7 @@
       <c r="AN32" s="8"/>
       <c r="AO32" s="8"/>
     </row>
-    <row r="33" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B33" s="30">
         <v>35855</v>
       </c>
@@ -3874,7 +3875,7 @@
       <c r="AN33" s="8"/>
       <c r="AO33" s="8"/>
     </row>
-    <row r="34" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B34" s="30">
         <v>35886</v>
       </c>
@@ -3962,7 +3963,7 @@
       <c r="AN34" s="8"/>
       <c r="AO34" s="8"/>
     </row>
-    <row r="35" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B35" s="30">
         <v>35916</v>
       </c>
@@ -4050,7 +4051,7 @@
       <c r="AN35" s="8"/>
       <c r="AO35" s="8"/>
     </row>
-    <row r="36" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B36" s="30">
         <v>35947</v>
       </c>
@@ -4138,7 +4139,7 @@
       <c r="AN36" s="8"/>
       <c r="AO36" s="8"/>
     </row>
-    <row r="37" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B37" s="30">
         <v>35977</v>
       </c>
@@ -4226,7 +4227,7 @@
       <c r="AN37" s="8"/>
       <c r="AO37" s="8"/>
     </row>
-    <row r="38" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B38" s="30">
         <v>36008</v>
       </c>
@@ -4314,7 +4315,7 @@
       <c r="AN38" s="8"/>
       <c r="AO38" s="8"/>
     </row>
-    <row r="39" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B39" s="30">
         <v>36039</v>
       </c>
@@ -4402,7 +4403,7 @@
       <c r="AN39" s="8"/>
       <c r="AO39" s="8"/>
     </row>
-    <row r="40" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B40" s="30">
         <v>36069</v>
       </c>
@@ -4490,7 +4491,7 @@
       <c r="AN40" s="8"/>
       <c r="AO40" s="8"/>
     </row>
-    <row r="41" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B41" s="30">
         <v>36100</v>
       </c>
@@ -4578,7 +4579,7 @@
       <c r="AN41" s="8"/>
       <c r="AO41" s="8"/>
     </row>
-    <row r="42" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B42" s="30">
         <v>36130</v>
       </c>
@@ -4666,7 +4667,7 @@
       <c r="AN42" s="8"/>
       <c r="AO42" s="8"/>
     </row>
-    <row r="43" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B43" s="30">
         <v>36161</v>
       </c>
@@ -4754,7 +4755,7 @@
       <c r="AN43" s="8"/>
       <c r="AO43" s="8"/>
     </row>
-    <row r="44" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B44" s="30">
         <v>36192</v>
       </c>
@@ -4842,7 +4843,7 @@
       <c r="AN44" s="8"/>
       <c r="AO44" s="8"/>
     </row>
-    <row r="45" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B45" s="30">
         <v>36220</v>
       </c>
@@ -4930,7 +4931,7 @@
       <c r="AN45" s="8"/>
       <c r="AO45" s="8"/>
     </row>
-    <row r="46" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B46" s="30">
         <v>36251</v>
       </c>
@@ -5018,7 +5019,7 @@
       <c r="AN46" s="8"/>
       <c r="AO46" s="8"/>
     </row>
-    <row r="47" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B47" s="30">
         <v>36281</v>
       </c>
@@ -5106,7 +5107,7 @@
       <c r="AN47" s="8"/>
       <c r="AO47" s="8"/>
     </row>
-    <row r="48" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B48" s="30">
         <v>36312</v>
       </c>
@@ -5194,7 +5195,7 @@
       <c r="AN48" s="8"/>
       <c r="AO48" s="8"/>
     </row>
-    <row r="49" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B49" s="30">
         <v>36342</v>
       </c>
@@ -5282,7 +5283,7 @@
       <c r="AN49" s="8"/>
       <c r="AO49" s="8"/>
     </row>
-    <row r="50" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B50" s="30">
         <v>36373</v>
       </c>
@@ -5370,7 +5371,7 @@
       <c r="AN50" s="8"/>
       <c r="AO50" s="8"/>
     </row>
-    <row r="51" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B51" s="30">
         <v>36404</v>
       </c>
@@ -5458,7 +5459,7 @@
       <c r="AN51" s="8"/>
       <c r="AO51" s="8"/>
     </row>
-    <row r="52" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B52" s="30">
         <v>36434</v>
       </c>
@@ -5546,7 +5547,7 @@
       <c r="AN52" s="8"/>
       <c r="AO52" s="8"/>
     </row>
-    <row r="53" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B53" s="30">
         <v>36465</v>
       </c>
@@ -5634,7 +5635,7 @@
       <c r="AN53" s="8"/>
       <c r="AO53" s="8"/>
     </row>
-    <row r="54" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B54" s="30">
         <v>36495</v>
       </c>
@@ -5722,7 +5723,7 @@
       <c r="AN54" s="8"/>
       <c r="AO54" s="8"/>
     </row>
-    <row r="55" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B55" s="30">
         <v>36526</v>
       </c>
@@ -5810,7 +5811,7 @@
       <c r="AN55" s="8"/>
       <c r="AO55" s="8"/>
     </row>
-    <row r="56" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B56" s="30">
         <v>36557</v>
       </c>
@@ -5898,7 +5899,7 @@
       <c r="AN56" s="8"/>
       <c r="AO56" s="8"/>
     </row>
-    <row r="57" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B57" s="30">
         <v>36586</v>
       </c>
@@ -5986,7 +5987,7 @@
       <c r="AN57" s="8"/>
       <c r="AO57" s="8"/>
     </row>
-    <row r="58" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B58" s="30">
         <v>36617</v>
       </c>
@@ -6074,7 +6075,7 @@
       <c r="AN58" s="8"/>
       <c r="AO58" s="8"/>
     </row>
-    <row r="59" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B59" s="30">
         <v>36647</v>
       </c>
@@ -6162,7 +6163,7 @@
       <c r="AN59" s="8"/>
       <c r="AO59" s="8"/>
     </row>
-    <row r="60" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B60" s="30">
         <v>36678</v>
       </c>
@@ -6250,7 +6251,7 @@
       <c r="AN60" s="8"/>
       <c r="AO60" s="8"/>
     </row>
-    <row r="61" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B61" s="30">
         <v>36708</v>
       </c>
@@ -6338,7 +6339,7 @@
       <c r="AN61" s="8"/>
       <c r="AO61" s="8"/>
     </row>
-    <row r="62" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B62" s="30">
         <v>36739</v>
       </c>
@@ -6426,7 +6427,7 @@
       <c r="AN62" s="8"/>
       <c r="AO62" s="8"/>
     </row>
-    <row r="63" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B63" s="30">
         <v>36770</v>
       </c>
@@ -6514,7 +6515,7 @@
       <c r="AN63" s="8"/>
       <c r="AO63" s="8"/>
     </row>
-    <row r="64" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B64" s="30">
         <v>36800</v>
       </c>
@@ -6602,7 +6603,7 @@
       <c r="AN64" s="8"/>
       <c r="AO64" s="8"/>
     </row>
-    <row r="65" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B65" s="30">
         <v>36831</v>
       </c>
@@ -6690,7 +6691,7 @@
       <c r="AN65" s="8"/>
       <c r="AO65" s="8"/>
     </row>
-    <row r="66" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B66" s="30">
         <v>36861</v>
       </c>
@@ -6778,7 +6779,7 @@
       <c r="AN66" s="8"/>
       <c r="AO66" s="8"/>
     </row>
-    <row r="67" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B67" s="30">
         <v>36892</v>
       </c>
@@ -6866,7 +6867,7 @@
       <c r="AN67" s="8"/>
       <c r="AO67" s="8"/>
     </row>
-    <row r="68" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B68" s="30">
         <v>36923</v>
       </c>
@@ -6954,7 +6955,7 @@
       <c r="AN68" s="8"/>
       <c r="AO68" s="8"/>
     </row>
-    <row r="69" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B69" s="30">
         <v>36951</v>
       </c>
@@ -7042,7 +7043,7 @@
       <c r="AN69" s="8"/>
       <c r="AO69" s="8"/>
     </row>
-    <row r="70" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B70" s="30">
         <v>36982</v>
       </c>
@@ -7130,7 +7131,7 @@
       <c r="AN70" s="8"/>
       <c r="AO70" s="8"/>
     </row>
-    <row r="71" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B71" s="30">
         <v>37012</v>
       </c>
@@ -7218,7 +7219,7 @@
       <c r="AN71" s="8"/>
       <c r="AO71" s="8"/>
     </row>
-    <row r="72" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B72" s="30">
         <v>37043</v>
       </c>
@@ -7306,7 +7307,7 @@
       <c r="AN72" s="8"/>
       <c r="AO72" s="8"/>
     </row>
-    <row r="73" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B73" s="30">
         <v>37073</v>
       </c>
@@ -7394,7 +7395,7 @@
       <c r="AN73" s="8"/>
       <c r="AO73" s="8"/>
     </row>
-    <row r="74" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B74" s="30">
         <v>37104</v>
       </c>
@@ -7482,7 +7483,7 @@
       <c r="AN74" s="8"/>
       <c r="AO74" s="8"/>
     </row>
-    <row r="75" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B75" s="30">
         <v>37135</v>
       </c>
@@ -7570,7 +7571,7 @@
       <c r="AN75" s="8"/>
       <c r="AO75" s="8"/>
     </row>
-    <row r="76" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B76" s="30">
         <v>37165</v>
       </c>
@@ -7658,7 +7659,7 @@
       <c r="AN76" s="8"/>
       <c r="AO76" s="8"/>
     </row>
-    <row r="77" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B77" s="30">
         <v>37196</v>
       </c>
@@ -7746,7 +7747,7 @@
       <c r="AN77" s="8"/>
       <c r="AO77" s="8"/>
     </row>
-    <row r="78" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B78" s="30">
         <v>37226</v>
       </c>
@@ -7834,7 +7835,7 @@
       <c r="AN78" s="8"/>
       <c r="AO78" s="8"/>
     </row>
-    <row r="79" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B79" s="30">
         <v>37257</v>
       </c>
@@ -7922,7 +7923,7 @@
       <c r="AN79" s="8"/>
       <c r="AO79" s="8"/>
     </row>
-    <row r="80" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B80" s="30">
         <v>37288</v>
       </c>
@@ -8010,7 +8011,7 @@
       <c r="AN80" s="8"/>
       <c r="AO80" s="8"/>
     </row>
-    <row r="81" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B81" s="30">
         <v>37316</v>
       </c>
@@ -8098,7 +8099,7 @@
       <c r="AN81" s="8"/>
       <c r="AO81" s="8"/>
     </row>
-    <row r="82" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B82" s="30">
         <v>37347</v>
       </c>
@@ -8186,7 +8187,7 @@
       <c r="AN82" s="8"/>
       <c r="AO82" s="8"/>
     </row>
-    <row r="83" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B83" s="30">
         <v>37377</v>
       </c>
@@ -8274,7 +8275,7 @@
       <c r="AN83" s="8"/>
       <c r="AO83" s="8"/>
     </row>
-    <row r="84" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B84" s="30">
         <v>37408</v>
       </c>
@@ -8362,7 +8363,7 @@
       <c r="AN84" s="8"/>
       <c r="AO84" s="8"/>
     </row>
-    <row r="85" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B85" s="30">
         <v>37438</v>
       </c>
@@ -8450,7 +8451,7 @@
       <c r="AN85" s="8"/>
       <c r="AO85" s="8"/>
     </row>
-    <row r="86" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B86" s="30">
         <v>37469</v>
       </c>
@@ -8538,7 +8539,7 @@
       <c r="AN86" s="8"/>
       <c r="AO86" s="8"/>
     </row>
-    <row r="87" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B87" s="30">
         <v>37500</v>
       </c>
@@ -8626,7 +8627,7 @@
       <c r="AN87" s="8"/>
       <c r="AO87" s="8"/>
     </row>
-    <row r="88" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B88" s="30">
         <v>37530</v>
       </c>
@@ -8714,7 +8715,7 @@
       <c r="AN88" s="8"/>
       <c r="AO88" s="8"/>
     </row>
-    <row r="89" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B89" s="30">
         <v>37561</v>
       </c>
@@ -8802,7 +8803,7 @@
       <c r="AN89" s="8"/>
       <c r="AO89" s="8"/>
     </row>
-    <row r="90" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B90" s="30">
         <v>37591</v>
       </c>
@@ -8890,7 +8891,7 @@
       <c r="AN90" s="8"/>
       <c r="AO90" s="8"/>
     </row>
-    <row r="91" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B91" s="30">
         <v>37622</v>
       </c>
@@ -8978,7 +8979,7 @@
       <c r="AN91" s="8"/>
       <c r="AO91" s="8"/>
     </row>
-    <row r="92" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B92" s="30">
         <v>37653</v>
       </c>
@@ -9066,7 +9067,7 @@
       <c r="AN92" s="8"/>
       <c r="AO92" s="8"/>
     </row>
-    <row r="93" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B93" s="30">
         <v>37681</v>
       </c>
@@ -9154,7 +9155,7 @@
       <c r="AN93" s="8"/>
       <c r="AO93" s="8"/>
     </row>
-    <row r="94" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B94" s="30">
         <v>37712</v>
       </c>
@@ -9242,7 +9243,7 @@
       <c r="AN94" s="8"/>
       <c r="AO94" s="8"/>
     </row>
-    <row r="95" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B95" s="30">
         <v>37742</v>
       </c>
@@ -9330,7 +9331,7 @@
       <c r="AN95" s="8"/>
       <c r="AO95" s="8"/>
     </row>
-    <row r="96" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B96" s="30">
         <v>37773</v>
       </c>
@@ -9418,7 +9419,7 @@
       <c r="AN96" s="8"/>
       <c r="AO96" s="8"/>
     </row>
-    <row r="97" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B97" s="30">
         <v>37803</v>
       </c>
@@ -9506,7 +9507,7 @@
       <c r="AN97" s="8"/>
       <c r="AO97" s="8"/>
     </row>
-    <row r="98" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B98" s="30">
         <v>37834</v>
       </c>
@@ -9594,7 +9595,7 @@
       <c r="AN98" s="8"/>
       <c r="AO98" s="8"/>
     </row>
-    <row r="99" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B99" s="30">
         <v>37865</v>
       </c>
@@ -9682,7 +9683,7 @@
       <c r="AN99" s="8"/>
       <c r="AO99" s="8"/>
     </row>
-    <row r="100" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B100" s="30">
         <v>37895</v>
       </c>
@@ -9770,7 +9771,7 @@
       <c r="AN100" s="8"/>
       <c r="AO100" s="8"/>
     </row>
-    <row r="101" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B101" s="30">
         <v>37926</v>
       </c>
@@ -9858,7 +9859,7 @@
       <c r="AN101" s="8"/>
       <c r="AO101" s="8"/>
     </row>
-    <row r="102" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B102" s="30">
         <v>37956</v>
       </c>
@@ -9946,7 +9947,7 @@
       <c r="AN102" s="8"/>
       <c r="AO102" s="8"/>
     </row>
-    <row r="103" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B103" s="30">
         <v>37987</v>
       </c>
@@ -10034,7 +10035,7 @@
       <c r="AN103" s="8"/>
       <c r="AO103" s="8"/>
     </row>
-    <row r="104" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B104" s="30">
         <v>38018</v>
       </c>
@@ -10122,7 +10123,7 @@
       <c r="AN104" s="8"/>
       <c r="AO104" s="8"/>
     </row>
-    <row r="105" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B105" s="30">
         <v>38047</v>
       </c>
@@ -10210,7 +10211,7 @@
       <c r="AN105" s="8"/>
       <c r="AO105" s="8"/>
     </row>
-    <row r="106" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B106" s="30">
         <v>38078</v>
       </c>
@@ -10298,7 +10299,7 @@
       <c r="AN106" s="8"/>
       <c r="AO106" s="8"/>
     </row>
-    <row r="107" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B107" s="30">
         <v>38108</v>
       </c>
@@ -10386,7 +10387,7 @@
       <c r="AN107" s="8"/>
       <c r="AO107" s="8"/>
     </row>
-    <row r="108" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B108" s="30">
         <v>38139</v>
       </c>
@@ -10474,7 +10475,7 @@
       <c r="AN108" s="8"/>
       <c r="AO108" s="8"/>
     </row>
-    <row r="109" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B109" s="30">
         <v>38169</v>
       </c>
@@ -10562,7 +10563,7 @@
       <c r="AN109" s="8"/>
       <c r="AO109" s="8"/>
     </row>
-    <row r="110" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B110" s="30">
         <v>38200</v>
       </c>
@@ -10650,7 +10651,7 @@
       <c r="AN110" s="8"/>
       <c r="AO110" s="8"/>
     </row>
-    <row r="111" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B111" s="30">
         <v>38231</v>
       </c>
@@ -10738,7 +10739,7 @@
       <c r="AN111" s="8"/>
       <c r="AO111" s="8"/>
     </row>
-    <row r="112" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B112" s="30">
         <v>38261</v>
       </c>
@@ -10826,7 +10827,7 @@
       <c r="AN112" s="8"/>
       <c r="AO112" s="8"/>
     </row>
-    <row r="113" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B113" s="30">
         <v>38292</v>
       </c>
@@ -10914,7 +10915,7 @@
       <c r="AN113" s="8"/>
       <c r="AO113" s="8"/>
     </row>
-    <row r="114" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B114" s="30">
         <v>38322</v>
       </c>
@@ -11002,7 +11003,7 @@
       <c r="AN114" s="8"/>
       <c r="AO114" s="8"/>
     </row>
-    <row r="115" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B115" s="30">
         <v>38353</v>
       </c>
@@ -11090,7 +11091,7 @@
       <c r="AN115" s="8"/>
       <c r="AO115" s="8"/>
     </row>
-    <row r="116" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B116" s="30">
         <v>38384</v>
       </c>
@@ -11178,7 +11179,7 @@
       <c r="AN116" s="8"/>
       <c r="AO116" s="8"/>
     </row>
-    <row r="117" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B117" s="30">
         <v>38412</v>
       </c>
@@ -11266,7 +11267,7 @@
       <c r="AN117" s="8"/>
       <c r="AO117" s="8"/>
     </row>
-    <row r="118" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B118" s="30">
         <v>38443</v>
       </c>
@@ -11354,7 +11355,7 @@
       <c r="AN118" s="8"/>
       <c r="AO118" s="8"/>
     </row>
-    <row r="119" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B119" s="30">
         <v>38473</v>
       </c>
@@ -11442,7 +11443,7 @@
       <c r="AN119" s="8"/>
       <c r="AO119" s="8"/>
     </row>
-    <row r="120" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B120" s="30">
         <v>38504</v>
       </c>
@@ -11530,7 +11531,7 @@
       <c r="AN120" s="8"/>
       <c r="AO120" s="8"/>
     </row>
-    <row r="121" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B121" s="30">
         <v>38534</v>
       </c>
@@ -11618,7 +11619,7 @@
       <c r="AN121" s="8"/>
       <c r="AO121" s="8"/>
     </row>
-    <row r="122" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B122" s="30">
         <v>38565</v>
       </c>
@@ -11706,7 +11707,7 @@
       <c r="AN122" s="8"/>
       <c r="AO122" s="8"/>
     </row>
-    <row r="123" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B123" s="30">
         <v>38596</v>
       </c>
@@ -11794,7 +11795,7 @@
       <c r="AN123" s="8"/>
       <c r="AO123" s="8"/>
     </row>
-    <row r="124" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B124" s="30">
         <v>38626</v>
       </c>
@@ -11882,7 +11883,7 @@
       <c r="AN124" s="8"/>
       <c r="AO124" s="8"/>
     </row>
-    <row r="125" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B125" s="30">
         <v>38657</v>
       </c>
@@ -11970,7 +11971,7 @@
       <c r="AN125" s="8"/>
       <c r="AO125" s="8"/>
     </row>
-    <row r="126" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B126" s="30">
         <v>38687</v>
       </c>
@@ -12058,7 +12059,7 @@
       <c r="AN126" s="8"/>
       <c r="AO126" s="8"/>
     </row>
-    <row r="127" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B127" s="30">
         <v>38718</v>
       </c>
@@ -12146,7 +12147,7 @@
       <c r="AN127" s="8"/>
       <c r="AO127" s="8"/>
     </row>
-    <row r="128" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="128" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B128" s="30">
         <v>38749</v>
       </c>
@@ -12234,7 +12235,7 @@
       <c r="AN128" s="8"/>
       <c r="AO128" s="8"/>
     </row>
-    <row r="129" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B129" s="30">
         <v>38777</v>
       </c>
@@ -12322,7 +12323,7 @@
       <c r="AN129" s="8"/>
       <c r="AO129" s="8"/>
     </row>
-    <row r="130" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B130" s="30">
         <v>38808</v>
       </c>
@@ -12410,7 +12411,7 @@
       <c r="AN130" s="8"/>
       <c r="AO130" s="8"/>
     </row>
-    <row r="131" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B131" s="30">
         <v>38838</v>
       </c>
@@ -12498,7 +12499,7 @@
       <c r="AN131" s="8"/>
       <c r="AO131" s="8"/>
     </row>
-    <row r="132" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B132" s="30">
         <v>38869</v>
       </c>
@@ -12586,7 +12587,7 @@
       <c r="AN132" s="8"/>
       <c r="AO132" s="8"/>
     </row>
-    <row r="133" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B133" s="30">
         <v>38899</v>
       </c>
@@ -12674,7 +12675,7 @@
       <c r="AN133" s="8"/>
       <c r="AO133" s="8"/>
     </row>
-    <row r="134" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B134" s="30">
         <v>38930</v>
       </c>
@@ -12762,7 +12763,7 @@
       <c r="AN134" s="8"/>
       <c r="AO134" s="8"/>
     </row>
-    <row r="135" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B135" s="30">
         <v>38961</v>
       </c>
@@ -12850,7 +12851,7 @@
       <c r="AN135" s="8"/>
       <c r="AO135" s="8"/>
     </row>
-    <row r="136" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B136" s="30">
         <v>38991</v>
       </c>
@@ -12938,7 +12939,7 @@
       <c r="AN136" s="8"/>
       <c r="AO136" s="8"/>
     </row>
-    <row r="137" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B137" s="30">
         <v>39022</v>
       </c>
@@ -13026,7 +13027,7 @@
       <c r="AN137" s="8"/>
       <c r="AO137" s="8"/>
     </row>
-    <row r="138" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B138" s="30">
         <v>39052</v>
       </c>
@@ -13114,7 +13115,7 @@
       <c r="AN138" s="8"/>
       <c r="AO138" s="8"/>
     </row>
-    <row r="139" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B139" s="30">
         <v>39083</v>
       </c>
@@ -13202,7 +13203,7 @@
       <c r="AN139" s="8"/>
       <c r="AO139" s="8"/>
     </row>
-    <row r="140" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B140" s="30">
         <v>39114</v>
       </c>
@@ -13290,7 +13291,7 @@
       <c r="AN140" s="8"/>
       <c r="AO140" s="8"/>
     </row>
-    <row r="141" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B141" s="30">
         <v>39142</v>
       </c>
@@ -13378,7 +13379,7 @@
       <c r="AN141" s="8"/>
       <c r="AO141" s="8"/>
     </row>
-    <row r="142" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B142" s="30">
         <v>39173</v>
       </c>
@@ -13466,7 +13467,7 @@
       <c r="AN142" s="8"/>
       <c r="AO142" s="8"/>
     </row>
-    <row r="143" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B143" s="30">
         <v>39203</v>
       </c>
@@ -13554,7 +13555,7 @@
       <c r="AN143" s="8"/>
       <c r="AO143" s="8"/>
     </row>
-    <row r="144" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B144" s="30">
         <v>39234</v>
       </c>
@@ -13642,7 +13643,7 @@
       <c r="AN144" s="8"/>
       <c r="AO144" s="8"/>
     </row>
-    <row r="145" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B145" s="30">
         <v>39264</v>
       </c>
@@ -13730,7 +13731,7 @@
       <c r="AN145" s="8"/>
       <c r="AO145" s="8"/>
     </row>
-    <row r="146" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B146" s="30">
         <v>39295</v>
       </c>
@@ -13818,7 +13819,7 @@
       <c r="AN146" s="8"/>
       <c r="AO146" s="8"/>
     </row>
-    <row r="147" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B147" s="30">
         <v>39326</v>
       </c>
@@ -13906,7 +13907,7 @@
       <c r="AN147" s="8"/>
       <c r="AO147" s="8"/>
     </row>
-    <row r="148" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B148" s="30">
         <v>39356</v>
       </c>
@@ -13994,7 +13995,7 @@
       <c r="AN148" s="8"/>
       <c r="AO148" s="8"/>
     </row>
-    <row r="149" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B149" s="30">
         <v>39387</v>
       </c>
@@ -14082,7 +14083,7 @@
       <c r="AN149" s="8"/>
       <c r="AO149" s="8"/>
     </row>
-    <row r="150" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B150" s="30">
         <v>39417</v>
       </c>
@@ -14170,7 +14171,7 @@
       <c r="AN150" s="8"/>
       <c r="AO150" s="8"/>
     </row>
-    <row r="151" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B151" s="30">
         <v>39448</v>
       </c>
@@ -14258,7 +14259,7 @@
       <c r="AN151" s="8"/>
       <c r="AO151" s="8"/>
     </row>
-    <row r="152" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B152" s="30">
         <v>39479</v>
       </c>
@@ -14346,7 +14347,7 @@
       <c r="AN152" s="8"/>
       <c r="AO152" s="8"/>
     </row>
-    <row r="153" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B153" s="30">
         <v>39508</v>
       </c>
@@ -14434,7 +14435,7 @@
       <c r="AN153" s="8"/>
       <c r="AO153" s="8"/>
     </row>
-    <row r="154" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="154" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B154" s="30">
         <v>39539</v>
       </c>
@@ -14522,7 +14523,7 @@
       <c r="AN154" s="8"/>
       <c r="AO154" s="8"/>
     </row>
-    <row r="155" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="155" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B155" s="30">
         <v>39569</v>
       </c>
@@ -14610,7 +14611,7 @@
       <c r="AN155" s="8"/>
       <c r="AO155" s="8"/>
     </row>
-    <row r="156" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="156" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B156" s="30">
         <v>39600</v>
       </c>
@@ -14698,7 +14699,7 @@
       <c r="AN156" s="8"/>
       <c r="AO156" s="8"/>
     </row>
-    <row r="157" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="157" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B157" s="30">
         <v>39630</v>
       </c>
@@ -14786,7 +14787,7 @@
       <c r="AN157" s="8"/>
       <c r="AO157" s="8"/>
     </row>
-    <row r="158" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="158" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B158" s="30">
         <v>39661</v>
       </c>
@@ -14874,7 +14875,7 @@
       <c r="AN158" s="8"/>
       <c r="AO158" s="8"/>
     </row>
-    <row r="159" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="159" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B159" s="30">
         <v>39692</v>
       </c>
@@ -14962,7 +14963,7 @@
       <c r="AN159" s="8"/>
       <c r="AO159" s="8"/>
     </row>
-    <row r="160" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="160" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B160" s="30">
         <v>39722</v>
       </c>
@@ -15050,7 +15051,7 @@
       <c r="AN160" s="8"/>
       <c r="AO160" s="8"/>
     </row>
-    <row r="161" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="161" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B161" s="30">
         <v>39753</v>
       </c>
@@ -15138,7 +15139,7 @@
       <c r="AN161" s="8"/>
       <c r="AO161" s="8"/>
     </row>
-    <row r="162" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="162" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B162" s="30">
         <v>39783</v>
       </c>
@@ -15226,7 +15227,7 @@
       <c r="AN162" s="8"/>
       <c r="AO162" s="8"/>
     </row>
-    <row r="163" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="163" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B163" s="30">
         <v>39814</v>
       </c>
@@ -15314,7 +15315,7 @@
       <c r="AN163" s="8"/>
       <c r="AO163" s="8"/>
     </row>
-    <row r="164" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="164" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B164" s="30">
         <v>39845</v>
       </c>
@@ -15402,7 +15403,7 @@
       <c r="AN164" s="8"/>
       <c r="AO164" s="8"/>
     </row>
-    <row r="165" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="165" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B165" s="30">
         <v>39873</v>
       </c>
@@ -15490,7 +15491,7 @@
       <c r="AN165" s="8"/>
       <c r="AO165" s="8"/>
     </row>
-    <row r="166" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="166" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B166" s="30">
         <v>39904</v>
       </c>
@@ -15578,7 +15579,7 @@
       <c r="AN166" s="8"/>
       <c r="AO166" s="8"/>
     </row>
-    <row r="167" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B167" s="30">
         <v>39934</v>
       </c>
@@ -15666,7 +15667,7 @@
       <c r="AN167" s="8"/>
       <c r="AO167" s="8"/>
     </row>
-    <row r="168" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="168" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B168" s="30">
         <v>39965</v>
       </c>
@@ -15754,7 +15755,7 @@
       <c r="AN168" s="8"/>
       <c r="AO168" s="8"/>
     </row>
-    <row r="169" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="169" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B169" s="30">
         <v>39995</v>
       </c>
@@ -15842,7 +15843,7 @@
       <c r="AN169" s="8"/>
       <c r="AO169" s="8"/>
     </row>
-    <row r="170" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="170" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B170" s="30">
         <v>40026</v>
       </c>
@@ -15930,7 +15931,7 @@
       <c r="AN170" s="8"/>
       <c r="AO170" s="8"/>
     </row>
-    <row r="171" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B171" s="30">
         <v>40057</v>
       </c>
@@ -16018,7 +16019,7 @@
       <c r="AN171" s="8"/>
       <c r="AO171" s="8"/>
     </row>
-    <row r="172" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="172" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B172" s="30">
         <v>40087</v>
       </c>
@@ -16106,7 +16107,7 @@
       <c r="AN172" s="8"/>
       <c r="AO172" s="8"/>
     </row>
-    <row r="173" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="173" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B173" s="30">
         <v>40118</v>
       </c>
@@ -16194,7 +16195,7 @@
       <c r="AN173" s="8"/>
       <c r="AO173" s="8"/>
     </row>
-    <row r="174" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="174" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B174" s="30">
         <v>40148</v>
       </c>
@@ -16282,7 +16283,7 @@
       <c r="AN174" s="8"/>
       <c r="AO174" s="8"/>
     </row>
-    <row r="175" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="175" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B175" s="30">
         <v>40179</v>
       </c>
@@ -16370,7 +16371,7 @@
       <c r="AN175" s="8"/>
       <c r="AO175" s="8"/>
     </row>
-    <row r="176" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="176" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B176" s="30">
         <v>40210</v>
       </c>
@@ -16458,7 +16459,7 @@
       <c r="AN176" s="8"/>
       <c r="AO176" s="8"/>
     </row>
-    <row r="177" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="177" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B177" s="30">
         <v>40238</v>
       </c>
@@ -16546,7 +16547,7 @@
       <c r="AN177" s="8"/>
       <c r="AO177" s="8"/>
     </row>
-    <row r="178" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="178" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B178" s="30">
         <v>40269</v>
       </c>
@@ -16634,7 +16635,7 @@
       <c r="AN178" s="8"/>
       <c r="AO178" s="8"/>
     </row>
-    <row r="179" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="179" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B179" s="30">
         <v>40299</v>
       </c>
@@ -16722,7 +16723,7 @@
       <c r="AN179" s="8"/>
       <c r="AO179" s="8"/>
     </row>
-    <row r="180" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="180" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B180" s="30">
         <v>40330</v>
       </c>
@@ -16810,7 +16811,7 @@
       <c r="AN180" s="8"/>
       <c r="AO180" s="8"/>
     </row>
-    <row r="181" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="181" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B181" s="30">
         <v>40360</v>
       </c>
@@ -16898,7 +16899,7 @@
       <c r="AN181" s="8"/>
       <c r="AO181" s="8"/>
     </row>
-    <row r="182" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="182" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B182" s="30">
         <v>40391</v>
       </c>
@@ -16986,7 +16987,7 @@
       <c r="AN182" s="8"/>
       <c r="AO182" s="8"/>
     </row>
-    <row r="183" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="183" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B183" s="30">
         <v>40422</v>
       </c>
@@ -17074,7 +17075,7 @@
       <c r="AN183" s="8"/>
       <c r="AO183" s="8"/>
     </row>
-    <row r="184" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="184" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B184" s="30">
         <v>40452</v>
       </c>
@@ -17162,7 +17163,7 @@
       <c r="AN184" s="8"/>
       <c r="AO184" s="8"/>
     </row>
-    <row r="185" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="185" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B185" s="30">
         <v>40483</v>
       </c>
@@ -17250,7 +17251,7 @@
       <c r="AN185" s="8"/>
       <c r="AO185" s="8"/>
     </row>
-    <row r="186" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B186" s="30">
         <v>40513</v>
       </c>
@@ -17338,7 +17339,7 @@
       <c r="AN186" s="8"/>
       <c r="AO186" s="8"/>
     </row>
-    <row r="187" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="187" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B187" s="30">
         <v>40544</v>
       </c>
@@ -17426,7 +17427,7 @@
       <c r="AN187" s="8"/>
       <c r="AO187" s="8"/>
     </row>
-    <row r="188" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="188" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B188" s="30">
         <v>40575</v>
       </c>
@@ -17514,7 +17515,7 @@
       <c r="AN188" s="8"/>
       <c r="AO188" s="8"/>
     </row>
-    <row r="189" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="189" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B189" s="30">
         <v>40603</v>
       </c>
@@ -17602,7 +17603,7 @@
       <c r="AN189" s="8"/>
       <c r="AO189" s="8"/>
     </row>
-    <row r="190" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="190" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B190" s="30">
         <v>40634</v>
       </c>
@@ -17690,7 +17691,7 @@
       <c r="AN190" s="8"/>
       <c r="AO190" s="8"/>
     </row>
-    <row r="191" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="191" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B191" s="30">
         <v>40664</v>
       </c>
@@ -17778,7 +17779,7 @@
       <c r="AN191" s="8"/>
       <c r="AO191" s="8"/>
     </row>
-    <row r="192" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="192" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B192" s="30">
         <v>40695</v>
       </c>
@@ -17866,7 +17867,7 @@
       <c r="AN192" s="8"/>
       <c r="AO192" s="8"/>
     </row>
-    <row r="193" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="193" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B193" s="30">
         <v>40725</v>
       </c>
@@ -17954,7 +17955,7 @@
       <c r="AN193" s="8"/>
       <c r="AO193" s="8"/>
     </row>
-    <row r="194" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="194" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B194" s="30">
         <v>40756</v>
       </c>
@@ -18042,7 +18043,7 @@
       <c r="AN194" s="8"/>
       <c r="AO194" s="8"/>
     </row>
-    <row r="195" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="195" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B195" s="30">
         <v>40787</v>
       </c>
@@ -18130,7 +18131,7 @@
       <c r="AN195" s="8"/>
       <c r="AO195" s="8"/>
     </row>
-    <row r="196" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="196" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B196" s="30">
         <v>40817</v>
       </c>
@@ -18218,7 +18219,7 @@
       <c r="AN196" s="8"/>
       <c r="AO196" s="8"/>
     </row>
-    <row r="197" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="197" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B197" s="30">
         <v>40848</v>
       </c>
@@ -18306,7 +18307,7 @@
       <c r="AN197" s="8"/>
       <c r="AO197" s="8"/>
     </row>
-    <row r="198" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="198" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B198" s="30">
         <v>40878</v>
       </c>
@@ -18394,7 +18395,7 @@
       <c r="AN198" s="8"/>
       <c r="AO198" s="8"/>
     </row>
-    <row r="199" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="199" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B199" s="30">
         <v>40909</v>
       </c>
@@ -18482,7 +18483,7 @@
       <c r="AN199" s="8"/>
       <c r="AO199" s="8"/>
     </row>
-    <row r="200" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="200" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B200" s="30">
         <v>40940</v>
       </c>
@@ -18570,7 +18571,7 @@
       <c r="AN200" s="8"/>
       <c r="AO200" s="8"/>
     </row>
-    <row r="201" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="201" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B201" s="30">
         <v>40969</v>
       </c>
@@ -18658,7 +18659,7 @@
       <c r="AN201" s="8"/>
       <c r="AO201" s="8"/>
     </row>
-    <row r="202" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="202" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B202" s="30">
         <v>41000</v>
       </c>
@@ -18746,7 +18747,7 @@
       <c r="AN202" s="8"/>
       <c r="AO202" s="8"/>
     </row>
-    <row r="203" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="203" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B203" s="30">
         <v>41030</v>
       </c>
@@ -18834,7 +18835,7 @@
       <c r="AN203" s="8"/>
       <c r="AO203" s="8"/>
     </row>
-    <row r="204" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="204" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B204" s="30">
         <v>41061</v>
       </c>
@@ -18922,7 +18923,7 @@
       <c r="AN204" s="8"/>
       <c r="AO204" s="8"/>
     </row>
-    <row r="205" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="205" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B205" s="30">
         <v>41091</v>
       </c>
@@ -19010,7 +19011,7 @@
       <c r="AN205" s="8"/>
       <c r="AO205" s="8"/>
     </row>
-    <row r="206" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="206" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B206" s="30">
         <v>41122</v>
       </c>
@@ -19098,7 +19099,7 @@
       <c r="AN206" s="8"/>
       <c r="AO206" s="8"/>
     </row>
-    <row r="207" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="207" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B207" s="30">
         <v>41153</v>
       </c>
@@ -19186,7 +19187,7 @@
       <c r="AN207" s="8"/>
       <c r="AO207" s="8"/>
     </row>
-    <row r="208" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="208" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B208" s="30">
         <v>41183</v>
       </c>
@@ -19274,7 +19275,7 @@
       <c r="AN208" s="8"/>
       <c r="AO208" s="8"/>
     </row>
-    <row r="209" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="209" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B209" s="30">
         <v>41214</v>
       </c>
@@ -19362,7 +19363,7 @@
       <c r="AN209" s="8"/>
       <c r="AO209" s="8"/>
     </row>
-    <row r="210" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="210" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B210" s="30">
         <v>41244</v>
       </c>
@@ -19450,7 +19451,7 @@
       <c r="AN210" s="8"/>
       <c r="AO210" s="8"/>
     </row>
-    <row r="211" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="211" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B211" s="30">
         <v>41275</v>
       </c>
@@ -19538,7 +19539,7 @@
       <c r="AN211" s="8"/>
       <c r="AO211" s="8"/>
     </row>
-    <row r="212" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="212" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B212" s="30">
         <v>41306</v>
       </c>
@@ -19626,7 +19627,7 @@
       <c r="AN212" s="8"/>
       <c r="AO212" s="8"/>
     </row>
-    <row r="213" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="213" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B213" s="30">
         <v>41334</v>
       </c>
@@ -19714,7 +19715,7 @@
       <c r="AN213" s="8"/>
       <c r="AO213" s="8"/>
     </row>
-    <row r="214" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="214" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B214" s="30">
         <v>41365</v>
       </c>
@@ -19802,7 +19803,7 @@
       <c r="AN214" s="8"/>
       <c r="AO214" s="8"/>
     </row>
-    <row r="215" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="215" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B215" s="30">
         <v>41395</v>
       </c>
@@ -19890,7 +19891,7 @@
       <c r="AN215" s="8"/>
       <c r="AO215" s="8"/>
     </row>
-    <row r="216" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="216" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B216" s="30">
         <v>41426</v>
       </c>
@@ -19978,7 +19979,7 @@
       <c r="AN216" s="8"/>
       <c r="AO216" s="8"/>
     </row>
-    <row r="217" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="217" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B217" s="30">
         <v>41456</v>
       </c>
@@ -20066,7 +20067,7 @@
       <c r="AN217" s="8"/>
       <c r="AO217" s="8"/>
     </row>
-    <row r="218" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="218" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B218" s="30">
         <v>41487</v>
       </c>
@@ -20154,7 +20155,7 @@
       <c r="AN218" s="8"/>
       <c r="AO218" s="8"/>
     </row>
-    <row r="219" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="219" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B219" s="30">
         <v>41518</v>
       </c>
@@ -20242,7 +20243,7 @@
       <c r="AN219" s="8"/>
       <c r="AO219" s="8"/>
     </row>
-    <row r="220" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B220" s="30">
         <v>41548</v>
       </c>
@@ -20330,7 +20331,7 @@
       <c r="AN220" s="8"/>
       <c r="AO220" s="8"/>
     </row>
-    <row r="221" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B221" s="30">
         <v>41579</v>
       </c>
@@ -20418,7 +20419,7 @@
       <c r="AN221" s="8"/>
       <c r="AO221" s="8"/>
     </row>
-    <row r="222" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="222" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B222" s="30">
         <v>41609</v>
       </c>
@@ -20506,7 +20507,7 @@
       <c r="AN222" s="8"/>
       <c r="AO222" s="8"/>
     </row>
-    <row r="223" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="223" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B223" s="30">
         <v>41640</v>
       </c>
@@ -20594,7 +20595,7 @@
       <c r="AN223" s="8"/>
       <c r="AO223" s="8"/>
     </row>
-    <row r="224" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="224" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B224" s="30">
         <v>41671</v>
       </c>
@@ -20682,7 +20683,7 @@
       <c r="AN224" s="8"/>
       <c r="AO224" s="8"/>
     </row>
-    <row r="225" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="225" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B225" s="30">
         <v>41699</v>
       </c>
@@ -20770,7 +20771,7 @@
       <c r="AN225" s="8"/>
       <c r="AO225" s="8"/>
     </row>
-    <row r="226" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="226" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B226" s="30">
         <v>41730</v>
       </c>
@@ -20858,7 +20859,7 @@
       <c r="AN226" s="8"/>
       <c r="AO226" s="8"/>
     </row>
-    <row r="227" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="227" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B227" s="30">
         <v>41760</v>
       </c>
@@ -20946,7 +20947,7 @@
       <c r="AN227" s="8"/>
       <c r="AO227" s="8"/>
     </row>
-    <row r="228" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="228" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B228" s="30">
         <v>41791</v>
       </c>
@@ -21034,7 +21035,7 @@
       <c r="AN228" s="8"/>
       <c r="AO228" s="8"/>
     </row>
-    <row r="229" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B229" s="30">
         <v>41821</v>
       </c>
@@ -21122,7 +21123,7 @@
       <c r="AN229" s="8"/>
       <c r="AO229" s="8"/>
     </row>
-    <row r="230" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="230" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B230" s="30">
         <v>41852</v>
       </c>
@@ -21210,7 +21211,7 @@
       <c r="AN230" s="8"/>
       <c r="AO230" s="8"/>
     </row>
-    <row r="231" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B231" s="30">
         <v>41883</v>
       </c>
@@ -21298,7 +21299,7 @@
       <c r="AN231" s="8"/>
       <c r="AO231" s="8"/>
     </row>
-    <row r="232" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="232" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B232" s="30">
         <v>41913</v>
       </c>
@@ -21386,7 +21387,7 @@
       <c r="AN232" s="8"/>
       <c r="AO232" s="8"/>
     </row>
-    <row r="233" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="233" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B233" s="30">
         <v>41944</v>
       </c>
@@ -21474,7 +21475,7 @@
       <c r="AN233" s="8"/>
       <c r="AO233" s="8"/>
     </row>
-    <row r="234" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="234" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B234" s="30">
         <v>41974</v>
       </c>
@@ -21562,7 +21563,7 @@
       <c r="AN234" s="8"/>
       <c r="AO234" s="8"/>
     </row>
-    <row r="235" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="235" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B235" s="30">
         <v>42005</v>
       </c>
@@ -21650,7 +21651,7 @@
       <c r="AN235" s="8"/>
       <c r="AO235" s="8"/>
     </row>
-    <row r="236" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="236" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B236" s="30">
         <v>42036</v>
       </c>
@@ -21738,7 +21739,7 @@
       <c r="AN236" s="8"/>
       <c r="AO236" s="8"/>
     </row>
-    <row r="237" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="237" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B237" s="30">
         <v>42064</v>
       </c>
@@ -21826,7 +21827,7 @@
       <c r="AN237" s="8"/>
       <c r="AO237" s="8"/>
     </row>
-    <row r="238" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="238" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B238" s="30">
         <v>42095</v>
       </c>
@@ -21914,7 +21915,7 @@
       <c r="AN238" s="8"/>
       <c r="AO238" s="8"/>
     </row>
-    <row r="239" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="239" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B239" s="30">
         <v>42125</v>
       </c>
@@ -22002,7 +22003,7 @@
       <c r="AN239" s="8"/>
       <c r="AO239" s="8"/>
     </row>
-    <row r="240" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B240" s="30">
         <v>42156</v>
       </c>
@@ -22090,7 +22091,7 @@
       <c r="AN240" s="8"/>
       <c r="AO240" s="8"/>
     </row>
-    <row r="241" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="241" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B241" s="30">
         <v>42186</v>
       </c>
@@ -22178,7 +22179,7 @@
       <c r="AN241" s="8"/>
       <c r="AO241" s="8"/>
     </row>
-    <row r="242" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="242" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B242" s="30">
         <v>42217</v>
       </c>
@@ -22266,7 +22267,7 @@
       <c r="AN242" s="8"/>
       <c r="AO242" s="8"/>
     </row>
-    <row r="243" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="243" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B243" s="30">
         <v>42248</v>
       </c>
@@ -22354,7 +22355,7 @@
       <c r="AN243" s="8"/>
       <c r="AO243" s="8"/>
     </row>
-    <row r="244" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="244" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B244" s="31" t="s">
         <v>41</v>
       </c>
@@ -22442,7 +22443,7 @@
       <c r="AN244" s="8"/>
       <c r="AO244" s="8"/>
     </row>
-    <row r="245" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="245" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B245" s="30">
         <v>42309</v>
       </c>
@@ -22530,7 +22531,7 @@
       <c r="AN245" s="8"/>
       <c r="AO245" s="8"/>
     </row>
-    <row r="246" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="246" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B246" s="30">
         <v>42339</v>
       </c>
@@ -22618,7 +22619,7 @@
       <c r="AN246" s="8"/>
       <c r="AO246" s="8"/>
     </row>
-    <row r="247" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="247" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B247" s="30">
         <v>42370</v>
       </c>
@@ -22706,7 +22707,7 @@
       <c r="AN247" s="8"/>
       <c r="AO247" s="8"/>
     </row>
-    <row r="248" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="248" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B248" s="30">
         <v>42401</v>
       </c>
@@ -22794,7 +22795,7 @@
       <c r="AN248" s="8"/>
       <c r="AO248" s="8"/>
     </row>
-    <row r="249" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="249" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B249" s="30">
         <v>42430</v>
       </c>
@@ -22882,7 +22883,7 @@
       <c r="AN249" s="8"/>
       <c r="AO249" s="8"/>
     </row>
-    <row r="250" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="250" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B250" s="30">
         <v>42461</v>
       </c>
@@ -22970,7 +22971,7 @@
       <c r="AN250" s="8"/>
       <c r="AO250" s="8"/>
     </row>
-    <row r="251" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="251" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B251" s="30">
         <v>42491</v>
       </c>
@@ -23058,7 +23059,7 @@
       <c r="AN251" s="8"/>
       <c r="AO251" s="8"/>
     </row>
-    <row r="252" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="252" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B252" s="30">
         <v>42522</v>
       </c>
@@ -23146,7 +23147,7 @@
       <c r="AN252" s="8"/>
       <c r="AO252" s="8"/>
     </row>
-    <row r="253" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="253" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B253" s="30">
         <v>42552</v>
       </c>
@@ -23234,7 +23235,7 @@
       <c r="AN253" s="8"/>
       <c r="AO253" s="8"/>
     </row>
-    <row r="254" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="254" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B254" s="30">
         <v>42583</v>
       </c>
@@ -23322,7 +23323,7 @@
       <c r="AN254" s="8"/>
       <c r="AO254" s="8"/>
     </row>
-    <row r="255" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="255" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B255" s="30">
         <v>42614</v>
       </c>
@@ -23410,7 +23411,7 @@
       <c r="AN255" s="8"/>
       <c r="AO255" s="8"/>
     </row>
-    <row r="256" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="256" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B256" s="30">
         <v>42644</v>
       </c>
@@ -23496,7 +23497,7 @@
       <c r="AN256" s="8"/>
       <c r="AO256" s="8"/>
     </row>
-    <row r="257" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="257" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B257" s="30">
         <v>42675</v>
       </c>
@@ -23584,7 +23585,7 @@
       <c r="AN257" s="8"/>
       <c r="AO257" s="8"/>
     </row>
-    <row r="258" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="258" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B258" s="30">
         <v>42705</v>
       </c>
@@ -23672,7 +23673,7 @@
       <c r="AN258" s="8"/>
       <c r="AO258" s="8"/>
     </row>
-    <row r="259" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="259" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B259" s="30">
         <v>42736</v>
       </c>
@@ -23760,7 +23761,7 @@
       <c r="AN259" s="8"/>
       <c r="AO259" s="8"/>
     </row>
-    <row r="260" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="260" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B260" s="30">
         <v>42767</v>
       </c>
@@ -23848,7 +23849,7 @@
       <c r="AN260" s="8"/>
       <c r="AO260" s="8"/>
     </row>
-    <row r="261" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="261" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B261" s="30">
         <v>42795</v>
       </c>
@@ -23936,7 +23937,7 @@
       <c r="AN261" s="8"/>
       <c r="AO261" s="8"/>
     </row>
-    <row r="262" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="262" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B262" s="30">
         <v>42826</v>
       </c>
@@ -24024,7 +24025,7 @@
       <c r="AN262" s="8"/>
       <c r="AO262" s="8"/>
     </row>
-    <row r="263" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="263" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B263" s="30">
         <v>42856</v>
       </c>
@@ -24112,7 +24113,7 @@
       <c r="AN263" s="8"/>
       <c r="AO263" s="8"/>
     </row>
-    <row r="264" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="264" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B264" s="30">
         <v>42887</v>
       </c>
@@ -24200,7 +24201,7 @@
       <c r="AN264" s="8"/>
       <c r="AO264" s="8"/>
     </row>
-    <row r="265" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="265" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B265" s="30">
         <v>42917</v>
       </c>
@@ -24288,7 +24289,7 @@
       <c r="AN265" s="8"/>
       <c r="AO265" s="8"/>
     </row>
-    <row r="266" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="266" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B266" s="30">
         <v>42948</v>
       </c>
@@ -24376,7 +24377,7 @@
       <c r="AN266" s="8"/>
       <c r="AO266" s="8"/>
     </row>
-    <row r="267" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="267" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B267" s="30">
         <v>42979</v>
       </c>
@@ -24464,7 +24465,7 @@
       <c r="AN267" s="8"/>
       <c r="AO267" s="8"/>
     </row>
-    <row r="268" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="268" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B268" s="30">
         <v>43009</v>
       </c>
@@ -24552,7 +24553,7 @@
       <c r="AN268" s="8"/>
       <c r="AO268" s="8"/>
     </row>
-    <row r="269" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="269" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B269" s="30">
         <v>43040</v>
       </c>
@@ -24640,7 +24641,7 @@
       <c r="AN269" s="8"/>
       <c r="AO269" s="8"/>
     </row>
-    <row r="270" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="270" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B270" s="30">
         <v>43070</v>
       </c>
@@ -24728,7 +24729,7 @@
       <c r="AN270" s="8"/>
       <c r="AO270" s="8"/>
     </row>
-    <row r="271" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="271" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B271" s="30">
         <v>43101</v>
       </c>
@@ -24816,7 +24817,7 @@
       <c r="AN271" s="8"/>
       <c r="AO271" s="8"/>
     </row>
-    <row r="272" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B272" s="30">
         <v>43132</v>
       </c>
@@ -24904,7 +24905,7 @@
       <c r="AN272" s="8"/>
       <c r="AO272" s="8"/>
     </row>
-    <row r="273" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="273" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B273" s="30">
         <v>43160</v>
       </c>
@@ -24992,7 +24993,7 @@
       <c r="AN273" s="8"/>
       <c r="AO273" s="8"/>
     </row>
-    <row r="274" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="274" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B274" s="30">
         <v>43191</v>
       </c>
@@ -25080,7 +25081,7 @@
       <c r="AN274" s="8"/>
       <c r="AO274" s="8"/>
     </row>
-    <row r="275" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="275" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B275" s="30">
         <v>43221</v>
       </c>
@@ -25168,7 +25169,7 @@
       <c r="AN275" s="8"/>
       <c r="AO275" s="8"/>
     </row>
-    <row r="276" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="276" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B276" s="30">
         <v>43252</v>
       </c>
@@ -25256,7 +25257,7 @@
       <c r="AN276" s="8"/>
       <c r="AO276" s="8"/>
     </row>
-    <row r="277" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="277" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B277" s="30">
         <v>43282</v>
       </c>
@@ -25344,7 +25345,7 @@
       <c r="AN277" s="8"/>
       <c r="AO277" s="8"/>
     </row>
-    <row r="278" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="278" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B278" s="30">
         <v>43313</v>
       </c>
@@ -25432,7 +25433,7 @@
       <c r="AN278" s="8"/>
       <c r="AO278" s="8"/>
     </row>
-    <row r="279" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="279" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B279" s="30">
         <v>43344</v>
       </c>
@@ -25520,7 +25521,7 @@
       <c r="AN279" s="8"/>
       <c r="AO279" s="8"/>
     </row>
-    <row r="280" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="280" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B280" s="30">
         <v>43374</v>
       </c>
@@ -25608,7 +25609,7 @@
       <c r="AN280" s="8"/>
       <c r="AO280" s="8"/>
     </row>
-    <row r="281" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="281" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B281" s="30">
         <v>43405</v>
       </c>
@@ -25696,7 +25697,7 @@
       <c r="AN281" s="8"/>
       <c r="AO281" s="8"/>
     </row>
-    <row r="282" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="282" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B282" s="30">
         <v>43435</v>
       </c>
@@ -25784,7 +25785,7 @@
       <c r="AN282" s="8"/>
       <c r="AO282" s="8"/>
     </row>
-    <row r="283" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="283" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B283" s="30">
         <v>43466</v>
       </c>
@@ -25872,7 +25873,7 @@
       <c r="AN283" s="8"/>
       <c r="AO283" s="8"/>
     </row>
-    <row r="284" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="284" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B284" s="30">
         <v>43497</v>
       </c>
@@ -25960,7 +25961,7 @@
       <c r="AN284" s="8"/>
       <c r="AO284" s="8"/>
     </row>
-    <row r="285" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="285" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B285" s="30">
         <v>43525</v>
       </c>
@@ -26048,7 +26049,7 @@
       <c r="AN285" s="8"/>
       <c r="AO285" s="8"/>
     </row>
-    <row r="286" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="286" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B286" s="30">
         <v>43556</v>
       </c>
@@ -26136,7 +26137,7 @@
       <c r="AN286" s="8"/>
       <c r="AO286" s="8"/>
     </row>
-    <row r="287" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B287" s="30">
         <v>43586</v>
       </c>
@@ -26224,7 +26225,7 @@
       <c r="AN287" s="8"/>
       <c r="AO287" s="8"/>
     </row>
-    <row r="288" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="288" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B288" s="30">
         <v>43617</v>
       </c>
@@ -26312,7 +26313,7 @@
       <c r="AN288" s="8"/>
       <c r="AO288" s="8"/>
     </row>
-    <row r="289" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="289" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B289" s="30">
         <v>43647</v>
       </c>
@@ -26400,7 +26401,7 @@
       <c r="AN289" s="8"/>
       <c r="AO289" s="8"/>
     </row>
-    <row r="290" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="290" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B290" s="30">
         <v>43678</v>
       </c>
@@ -26488,7 +26489,7 @@
       <c r="AN290" s="8"/>
       <c r="AO290" s="8"/>
     </row>
-    <row r="291" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="291" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B291" s="30">
         <v>43709</v>
       </c>
@@ -26576,7 +26577,7 @@
       <c r="AN291" s="8"/>
       <c r="AO291" s="8"/>
     </row>
-    <row r="292" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="292" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B292" s="30">
         <v>43739</v>
       </c>
@@ -26664,7 +26665,7 @@
       <c r="AN292" s="8"/>
       <c r="AO292" s="8"/>
     </row>
-    <row r="293" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="293" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B293" s="30">
         <v>43770</v>
       </c>
@@ -26752,7 +26753,7 @@
       <c r="AN293" s="8"/>
       <c r="AO293" s="8"/>
     </row>
-    <row r="294" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="294" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B294" s="30">
         <v>43800</v>
       </c>
@@ -26840,7 +26841,7 @@
       <c r="AN294" s="8"/>
       <c r="AO294" s="8"/>
     </row>
-    <row r="295" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="295" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B295" s="30">
         <v>43831</v>
       </c>
@@ -26928,7 +26929,7 @@
       <c r="AN295" s="8"/>
       <c r="AO295" s="8"/>
     </row>
-    <row r="296" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="296" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B296" s="30">
         <v>43862</v>
       </c>
@@ -27016,7 +27017,7 @@
       <c r="AN296" s="8"/>
       <c r="AO296" s="8"/>
     </row>
-    <row r="297" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="297" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B297" s="30">
         <v>43891</v>
       </c>
@@ -27104,7 +27105,7 @@
       <c r="AN297" s="8"/>
       <c r="AO297" s="8"/>
     </row>
-    <row r="298" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="298" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B298" s="30">
         <v>43922</v>
       </c>
@@ -27192,7 +27193,7 @@
       <c r="AN298" s="8"/>
       <c r="AO298" s="8"/>
     </row>
-    <row r="299" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="299" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B299" s="30">
         <v>43952</v>
       </c>
@@ -27280,7 +27281,7 @@
       <c r="AN299" s="8"/>
       <c r="AO299" s="8"/>
     </row>
-    <row r="300" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="300" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B300" s="30">
         <v>43983</v>
       </c>
@@ -27368,7 +27369,7 @@
       <c r="AN300" s="8"/>
       <c r="AO300" s="8"/>
     </row>
-    <row r="301" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="301" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B301" s="30">
         <v>44013</v>
       </c>
@@ -27456,7 +27457,7 @@
       <c r="AN301" s="8"/>
       <c r="AO301" s="8"/>
     </row>
-    <row r="302" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="302" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B302" s="30">
         <v>44044</v>
       </c>
@@ -27544,7 +27545,7 @@
       <c r="AN302" s="8"/>
       <c r="AO302" s="8"/>
     </row>
-    <row r="303" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B303" s="30">
         <v>44075</v>
       </c>
@@ -27632,7 +27633,7 @@
       <c r="AN303" s="8"/>
       <c r="AO303" s="8"/>
     </row>
-    <row r="304" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="304" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B304" s="30">
         <v>44105</v>
       </c>
@@ -27720,7 +27721,7 @@
       <c r="AN304" s="8"/>
       <c r="AO304" s="8"/>
     </row>
-    <row r="305" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="305" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B305" s="30">
         <v>44136</v>
       </c>
@@ -27808,7 +27809,7 @@
       <c r="AN305" s="8"/>
       <c r="AO305" s="8"/>
     </row>
-    <row r="306" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="306" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B306" s="30">
         <v>44166</v>
       </c>
@@ -27896,7 +27897,7 @@
       <c r="AN306" s="8"/>
       <c r="AO306" s="8"/>
     </row>
-    <row r="307" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="307" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B307" s="30">
         <v>44197</v>
       </c>
@@ -27984,7 +27985,7 @@
       <c r="AN307" s="8"/>
       <c r="AO307" s="8"/>
     </row>
-    <row r="308" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="308" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B308" s="30">
         <v>44228</v>
       </c>
@@ -28072,7 +28073,7 @@
       <c r="AN308" s="8"/>
       <c r="AO308" s="8"/>
     </row>
-    <row r="309" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="309" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B309" s="30">
         <v>44256</v>
       </c>
@@ -28160,7 +28161,7 @@
       <c r="AN309" s="8"/>
       <c r="AO309" s="8"/>
     </row>
-    <row r="310" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="310" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B310" s="30">
         <v>44287</v>
       </c>
@@ -28248,7 +28249,7 @@
       <c r="AN310" s="8"/>
       <c r="AO310" s="8"/>
     </row>
-    <row r="311" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="311" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B311" s="30">
         <v>44317</v>
       </c>
@@ -28336,7 +28337,7 @@
       <c r="AN311" s="8"/>
       <c r="AO311" s="8"/>
     </row>
-    <row r="312" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="312" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B312" s="30">
         <v>44348</v>
       </c>
@@ -28424,7 +28425,7 @@
       <c r="AN312" s="8"/>
       <c r="AO312" s="8"/>
     </row>
-    <row r="313" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="313" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B313" s="30">
         <v>44378</v>
       </c>
@@ -28512,7 +28513,7 @@
       <c r="AN313" s="8"/>
       <c r="AO313" s="8"/>
     </row>
-    <row r="314" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="314" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B314" s="30">
         <v>44409</v>
       </c>
@@ -28600,7 +28601,7 @@
       <c r="AN314" s="8"/>
       <c r="AO314" s="8"/>
     </row>
-    <row r="315" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B315" s="30">
         <v>44440</v>
       </c>
@@ -28688,7 +28689,7 @@
       <c r="AN315" s="8"/>
       <c r="AO315" s="8"/>
     </row>
-    <row r="316" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B316" s="30">
         <v>44470</v>
       </c>
@@ -28776,7 +28777,7 @@
       <c r="AN316" s="8"/>
       <c r="AO316" s="8"/>
     </row>
-    <row r="317" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B317" s="30">
         <v>44501</v>
       </c>
@@ -28864,7 +28865,7 @@
       <c r="AN317" s="8"/>
       <c r="AO317" s="8"/>
     </row>
-    <row r="318" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B318" s="30">
         <v>44531</v>
       </c>
@@ -28952,7 +28953,7 @@
       <c r="AN318" s="8"/>
       <c r="AO318" s="8"/>
     </row>
-    <row r="319" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B319" s="41">
         <v>44583</v>
       </c>
@@ -29040,7 +29041,7 @@
       <c r="AN319" s="8"/>
       <c r="AO319" s="8"/>
     </row>
-    <row r="320" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B320" s="41">
         <v>44614</v>
       </c>
@@ -29128,7 +29129,7 @@
       <c r="AN320" s="8"/>
       <c r="AO320" s="8"/>
     </row>
-    <row r="321" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B321" s="41">
         <v>44642</v>
       </c>
@@ -29216,7 +29217,7 @@
       <c r="AN321" s="8"/>
       <c r="AO321" s="8"/>
     </row>
-    <row r="322" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B322" s="41">
         <v>44673</v>
       </c>
@@ -29304,7 +29305,7 @@
       <c r="AN322" s="8"/>
       <c r="AO322" s="8"/>
     </row>
-    <row r="323" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B323" s="41">
         <v>44703</v>
       </c>
@@ -29392,7 +29393,7 @@
       <c r="AN323" s="8"/>
       <c r="AO323" s="8"/>
     </row>
-    <row r="324" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B324" s="41">
         <v>44734</v>
       </c>
@@ -29480,7 +29481,7 @@
       <c r="AN324" s="8"/>
       <c r="AO324" s="8"/>
     </row>
-    <row r="325" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B325" s="41">
         <v>44764</v>
       </c>
@@ -29568,7 +29569,7 @@
       <c r="AN325" s="8"/>
       <c r="AO325" s="8"/>
     </row>
-    <row r="326" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B326" s="41">
         <v>44795</v>
       </c>
@@ -29656,7 +29657,7 @@
       <c r="AN326" s="8"/>
       <c r="AO326" s="8"/>
     </row>
-    <row r="327" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B327" s="41">
         <v>44826</v>
       </c>
@@ -29744,7 +29745,7 @@
       <c r="AN327" s="8"/>
       <c r="AO327" s="8"/>
     </row>
-    <row r="328" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B328" s="41">
         <v>44856</v>
       </c>
@@ -29832,7 +29833,7 @@
       <c r="AN328" s="8"/>
       <c r="AO328" s="8"/>
     </row>
-    <row r="329" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B329" s="41">
         <v>44887</v>
       </c>
@@ -29920,7 +29921,7 @@
       <c r="AN329" s="8"/>
       <c r="AO329" s="8"/>
     </row>
-    <row r="330" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B330" s="41">
         <v>44917</v>
       </c>
@@ -30008,7 +30009,7 @@
       <c r="AN330" s="8"/>
       <c r="AO330" s="8"/>
     </row>
-    <row r="331" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B331" s="41">
         <v>44948</v>
       </c>
@@ -30096,7 +30097,7 @@
       <c r="AN331" s="8"/>
       <c r="AO331" s="8"/>
     </row>
-    <row r="332" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B332" s="41">
         <v>44979</v>
       </c>
@@ -30184,7 +30185,7 @@
       <c r="AN332" s="8"/>
       <c r="AO332" s="8"/>
     </row>
-    <row r="333" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B333" s="41">
         <v>45008</v>
       </c>
@@ -30272,7 +30273,7 @@
       <c r="AN333" s="8"/>
       <c r="AO333" s="8"/>
     </row>
-    <row r="334" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B334" s="41" t="s">
         <v>40</v>
       </c>
@@ -30360,7 +30361,7 @@
       <c r="AN334" s="8"/>
       <c r="AO334" s="8"/>
     </row>
-    <row r="335" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B335" s="41">
         <v>45069</v>
       </c>
@@ -30448,7 +30449,7 @@
       <c r="AN335" s="8"/>
       <c r="AO335" s="8"/>
     </row>
-    <row r="336" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B336" s="41">
         <v>45099</v>
       </c>
@@ -30536,7 +30537,7 @@
       <c r="AN336" s="8"/>
       <c r="AO336" s="8"/>
     </row>
-    <row r="337" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B337" s="41">
         <v>45129</v>
       </c>
@@ -30624,7 +30625,7 @@
       <c r="AN337" s="8"/>
       <c r="AO337" s="8"/>
     </row>
-    <row r="338" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B338" s="41">
         <v>45160</v>
       </c>
@@ -30712,7 +30713,7 @@
       <c r="AN338" s="8"/>
       <c r="AO338" s="8"/>
     </row>
-    <row r="339" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B339" s="41">
         <v>45192</v>
       </c>
@@ -30800,7 +30801,7 @@
       <c r="AN339" s="8"/>
       <c r="AO339" s="8"/>
     </row>
-    <row r="340" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B340" s="41">
         <v>45221</v>
       </c>
@@ -30888,7 +30889,7 @@
       <c r="AN340" s="8"/>
       <c r="AO340" s="8"/>
     </row>
-    <row r="341" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B341" s="41">
         <v>45252</v>
       </c>
@@ -30976,7 +30977,7 @@
       <c r="AN341" s="8"/>
       <c r="AO341" s="8"/>
     </row>
-    <row r="342" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B342" s="41" t="s">
         <v>39</v>
       </c>
@@ -31064,7 +31065,7 @@
       <c r="AN342" s="8"/>
       <c r="AO342" s="8"/>
     </row>
-    <row r="343" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B343" s="41">
         <v>45292</v>
       </c>
@@ -31152,7 +31153,7 @@
       <c r="AN343" s="8"/>
       <c r="AO343" s="8"/>
     </row>
-    <row r="344" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B344" s="41">
         <v>45323</v>
       </c>
@@ -31240,7 +31241,7 @@
       <c r="AN344" s="8"/>
       <c r="AO344" s="8"/>
     </row>
-    <row r="345" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B345" s="41">
         <v>45352</v>
       </c>
@@ -31328,7 +31329,7 @@
       <c r="AN345" s="8"/>
       <c r="AO345" s="8"/>
     </row>
-    <row r="346" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B346" s="41">
         <v>45383</v>
       </c>
@@ -31416,7 +31417,7 @@
       <c r="AN346" s="8"/>
       <c r="AO346" s="8"/>
     </row>
-    <row r="347" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B347" s="41">
         <v>45413</v>
       </c>
@@ -31504,7 +31505,7 @@
       <c r="AN347" s="8"/>
       <c r="AO347" s="8"/>
     </row>
-    <row r="348" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B348" s="41">
         <v>45444</v>
       </c>
@@ -31592,7 +31593,7 @@
       <c r="AN348" s="8"/>
       <c r="AO348" s="8"/>
     </row>
-    <row r="349" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B349" s="41">
         <v>45474</v>
       </c>
@@ -31680,7 +31681,7 @@
       <c r="AN349" s="8"/>
       <c r="AO349" s="8"/>
     </row>
-    <row r="350" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B350" s="41">
         <v>45505</v>
       </c>
@@ -31768,7 +31769,7 @@
       <c r="AN350" s="8"/>
       <c r="AO350" s="8"/>
     </row>
-    <row r="351" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B351" s="41">
         <v>45536</v>
       </c>
@@ -31856,7 +31857,7 @@
       <c r="AN351" s="8"/>
       <c r="AO351" s="8"/>
     </row>
-    <row r="352" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B352" s="41">
         <v>45566</v>
       </c>
@@ -31944,7 +31945,7 @@
       <c r="AN352" s="8"/>
       <c r="AO352" s="8"/>
     </row>
-    <row r="353" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B353" s="41">
         <v>45597</v>
       </c>
@@ -31983,7 +31984,7 @@
         <f t="shared" si="66"/>
         <v>438240.38755505253</v>
       </c>
-      <c r="O353" s="65" t="s">
+      <c r="O353" s="62" t="s">
         <v>45</v>
       </c>
       <c r="P353" s="56">
@@ -32031,7 +32032,7 @@
       <c r="AN353" s="8"/>
       <c r="AO353" s="8"/>
     </row>
-    <row r="354" spans="2:41" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="2:41" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B354" s="58" t="s">
         <v>44</v>
       </c>
@@ -32119,7 +32120,7 @@
       <c r="AN354" s="8"/>
       <c r="AO354" s="8"/>
     </row>
-    <row r="355" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="355" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B355" s="42"/>
       <c r="C355" s="26"/>
       <c r="D355" s="26"/>
@@ -32179,68 +32180,68 @@
       <c r="T358" s="52"/>
     </row>
     <row r="359" spans="2:41" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B359" s="64" t="s">
+      <c r="B359" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C359" s="64"/>
-      <c r="D359" s="64"/>
-      <c r="E359" s="64"/>
-      <c r="F359" s="64"/>
-      <c r="G359" s="64"/>
-      <c r="H359" s="64"/>
-      <c r="I359" s="64"/>
-      <c r="J359" s="64"/>
-      <c r="K359" s="64"/>
-      <c r="L359" s="64"/>
-      <c r="M359" s="64"/>
-      <c r="N359" s="64"/>
-      <c r="O359" s="64"/>
-      <c r="P359" s="64"/>
-      <c r="Q359" s="64"/>
-      <c r="R359" s="64"/>
-      <c r="S359" s="64"/>
-      <c r="T359" s="64"/>
-      <c r="U359" s="64"/>
-      <c r="V359" s="64"/>
-      <c r="W359" s="64"/>
-    </row>
-    <row r="360" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="C359" s="65"/>
+      <c r="D359" s="65"/>
+      <c r="E359" s="65"/>
+      <c r="F359" s="65"/>
+      <c r="G359" s="65"/>
+      <c r="H359" s="65"/>
+      <c r="I359" s="65"/>
+      <c r="J359" s="65"/>
+      <c r="K359" s="65"/>
+      <c r="L359" s="65"/>
+      <c r="M359" s="65"/>
+      <c r="N359" s="65"/>
+      <c r="O359" s="65"/>
+      <c r="P359" s="65"/>
+      <c r="Q359" s="65"/>
+      <c r="R359" s="65"/>
+      <c r="S359" s="65"/>
+      <c r="T359" s="65"/>
+      <c r="U359" s="65"/>
+      <c r="V359" s="65"/>
+      <c r="W359" s="65"/>
+    </row>
+    <row r="360" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B360" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="361" spans="2:41" x14ac:dyDescent="0.3">
+    <row r="361" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B361" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="362" spans="2:41" ht="55.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B362" s="64" t="s">
+      <c r="B362" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="C362" s="64"/>
-      <c r="D362" s="64"/>
-      <c r="E362" s="64"/>
-      <c r="F362" s="64"/>
-      <c r="G362" s="64"/>
-      <c r="H362" s="64"/>
-      <c r="I362" s="64"/>
-      <c r="J362" s="64"/>
-      <c r="K362" s="64"/>
-      <c r="L362" s="64"/>
-      <c r="M362" s="64"/>
-      <c r="N362" s="64"/>
-      <c r="O362" s="64"/>
-      <c r="P362" s="64"/>
-      <c r="Q362" s="64"/>
-      <c r="R362" s="64"/>
-      <c r="S362" s="64"/>
-      <c r="T362" s="64"/>
-      <c r="U362" s="64"/>
-      <c r="V362" s="64"/>
-      <c r="W362" s="64"/>
-    </row>
-    <row r="363" spans="2:41" x14ac:dyDescent="0.3">
+      <c r="C362" s="65"/>
+      <c r="D362" s="65"/>
+      <c r="E362" s="65"/>
+      <c r="F362" s="65"/>
+      <c r="G362" s="65"/>
+      <c r="H362" s="65"/>
+      <c r="I362" s="65"/>
+      <c r="J362" s="65"/>
+      <c r="K362" s="65"/>
+      <c r="L362" s="65"/>
+      <c r="M362" s="65"/>
+      <c r="N362" s="65"/>
+      <c r="O362" s="65"/>
+      <c r="P362" s="65"/>
+      <c r="Q362" s="65"/>
+      <c r="R362" s="65"/>
+      <c r="S362" s="65"/>
+      <c r="T362" s="65"/>
+      <c r="U362" s="65"/>
+      <c r="V362" s="65"/>
+      <c r="W362" s="65"/>
+    </row>
+    <row r="363" spans="2:41" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B363" s="61" t="s">
         <v>42</v>
       </c>
@@ -32320,6 +32321,7 @@
       <c r="D376" s="8"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:D354" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <mergeCells count="4">
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="D4:D5"/>
@@ -32341,16 +32343,16 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.140625" customWidth="1"/>
-    <col min="2" max="2" width="64.42578125" customWidth="1"/>
-    <col min="3" max="3" width="1.5703125" customWidth="1"/>
-    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="1" max="1" width="1.109375" customWidth="1"/>
+    <col min="2" max="2" width="64.44140625" customWidth="1"/>
+    <col min="3" max="3" width="1.5546875" customWidth="1"/>
+    <col min="4" max="4" width="5.5546875" customWidth="1"/>
     <col min="5" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B1" s="13" t="s">
         <v>7</v>
       </c>
@@ -32359,7 +32361,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
@@ -32368,14 +32370,14 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" s="14"/>
       <c r="C3" s="14"/>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
     </row>
-    <row r="4" spans="2:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
         <v>9</v>
       </c>
@@ -32384,14 +32386,14 @@
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="14"/>
       <c r="C5" s="14"/>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="13" t="s">
         <v>10</v>
       </c>
@@ -32404,14 +32406,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
     </row>
-    <row r="8" spans="2:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>13</v>
       </c>
@@ -32424,14 +32426,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" s="14"/>
       <c r="C9" s="14"/>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B10" s="14"/>
       <c r="C10" s="14"/>
       <c r="D10" s="18"/>

</xml_diff>